<commit_message>
Chapter 3 dates included
</commit_message>
<xml_diff>
--- a/assets/ancient_india_timeline/timeline raw data.xlsx
+++ b/assets/ancient_india_timeline/timeline raw data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\V2QT9I3\Documents\Personal\Studies\home\assets\ancient_india_timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A4CFF4-4464-4772-84B8-F9521CB226EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE708882-9AAB-441C-BDB6-AE3988A0E5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16890" yWindow="-15780" windowWidth="20910" windowHeight="13065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Description</t>
   </si>
@@ -61,6 +61,81 @@
   </si>
   <si>
     <t>Yajur Veda, Atharva Veda, the Brahmanas, Aranyakas, and the Upanishads.</t>
+  </si>
+  <si>
+    <t>Shrautasutras and Grihyasutras.</t>
+  </si>
+  <si>
+    <t>Mahavira and the Buddha as per literature.</t>
+  </si>
+  <si>
+    <t>Dharmasutras.</t>
+  </si>
+  <si>
+    <t>Grammar of Panini.</t>
+  </si>
+  <si>
+    <t>Mahavira and the Buddha in the context of archaeology.</t>
+  </si>
+  <si>
+    <t>Alexander’s invasion.</t>
+  </si>
+  <si>
+    <t>Accession of Chandragupta Maurya.</t>
+  </si>
+  <si>
+    <t>Decipherable writing in India.</t>
+  </si>
+  <si>
+    <t>Vikrama Samvat.</t>
+  </si>
+  <si>
+    <t>Hathigumpha inscription of Kharavela of Kalinga.</t>
+  </si>
+  <si>
+    <t>The earliest Pali Buddhist texts compiled in Sri Lanka.</t>
+  </si>
+  <si>
+    <t>The Arthashastra of Kautilya finally compiled.</t>
+  </si>
+  <si>
+    <t>Start of Shaka Samvat.</t>
+  </si>
+  <si>
+    <t>The Periplus of the Erythrean Sea.</t>
+  </si>
+  <si>
+    <t>Ptolemy’s Geography.</t>
+  </si>
+  <si>
+    <t>Start of the Gupta era.</t>
+  </si>
+  <si>
+    <t>Mahabharata, Ramayana, and major Puranas finally compiled.</t>
+  </si>
+  <si>
+    <t>Earliest Indian manuscript found in Central Asia.</t>
+  </si>
+  <si>
+    <t>Fa-hsien comes to India.</t>
+  </si>
+  <si>
+    <t>The Prakrit Jaina texts finally compiled in Valabhi.</t>
+  </si>
+  <si>
+    <t>Hsuan Tsang’s visit. Harshacharita by Banabhatta.</t>
+  </si>
+  <si>
+    <t>Mushika Vamsha by Atula.</t>
+  </si>
+  <si>
+    <t>Vikramankadevacharita by Bilhana.</t>
+  </si>
+  <si>
+    <t>Ramacharita by Sandhyakara Nandi. Rajatarangini by Kalhana.</t>
+  </si>
+  <si>
+    <t>Ashokan inscriptions first deciphered by James Prinsep.</t>
   </si>
 </sst>
 </file>
@@ -378,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -484,7 +559,220 @@
         <v>11</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>-600</v>
+      </c>
+      <c r="B10">
+        <v>-300</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>-600</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>-500</v>
+      </c>
+      <c r="B12">
+        <v>-200</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>-450</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>-500</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>-326</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>-322</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>-300</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>-57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>-100</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>-100</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>100</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>78</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>80</v>
+      </c>
+      <c r="B23">
+        <v>115</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>150</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>319</v>
+      </c>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>400</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>400</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>500</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>600</v>
+      </c>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>700</v>
+      </c>
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>1100</v>
+      </c>
+      <c r="C31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>1100</v>
+      </c>
+      <c r="B32">
+        <v>1200</v>
+      </c>
+      <c r="C32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>1200</v>
+      </c>
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>1837</v>
+      </c>
+      <c r="C34" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Chapter 4 and 5 included
</commit_message>
<xml_diff>
--- a/assets/ancient_india_timeline/timeline raw data.xlsx
+++ b/assets/ancient_india_timeline/timeline raw data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\V2QT9I3\Documents\Personal\Studies\home\assets\ancient_india_timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE708882-9AAB-441C-BDB6-AE3988A0E5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543AF8DE-E33E-4C60-B8D0-BD5BCB708579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16890" yWindow="-15780" windowWidth="20910" windowHeight="13065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Description</t>
   </si>
@@ -136,6 +136,27 @@
   </si>
   <si>
     <t>Ashokan inscriptions first deciphered by James Prinsep.</t>
+  </si>
+  <si>
+    <t>Early trace of gold in Karnataka.</t>
+  </si>
+  <si>
+    <t>Earliest date of the Khetri copper belts.</t>
+  </si>
+  <si>
+    <t>Discovery of the direction of the monsoon.</t>
+  </si>
+  <si>
+    <t>Wide use of iron tools in the Gangetic plains and spurt in settlements.</t>
+  </si>
+  <si>
+    <t>Famine and Jain migration from Magadha to south India.</t>
+  </si>
+  <si>
+    <t>Forests in the Ganga-Yamuna doab despite deforestation.</t>
+  </si>
+  <si>
+    <t>The term Ecology coined.</t>
   </si>
 </sst>
 </file>
@@ -453,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -771,6 +792,65 @@
         <v>36</v>
       </c>
     </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>-1800</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>-1000</v>
+      </c>
+      <c r="C36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>100</v>
+      </c>
+      <c r="C37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>-500</v>
+      </c>
+      <c r="C38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>-300</v>
+      </c>
+      <c r="C39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>1600</v>
+      </c>
+      <c r="B40">
+        <v>1700</v>
+      </c>
+      <c r="C40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>1869</v>
+      </c>
+      <c r="C41" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Chapter 6 included. Uptodate with Kindle progress
</commit_message>
<xml_diff>
--- a/assets/ancient_india_timeline/timeline raw data.xlsx
+++ b/assets/ancient_india_timeline/timeline raw data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\V2QT9I3\Documents\Personal\Studies\home\assets\ancient_india_timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543AF8DE-E33E-4C60-B8D0-BD5BCB708579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED855DE-123F-45FB-9DA6-97CBBD596B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16890" yWindow="-15780" windowWidth="20910" windowHeight="13065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Description</t>
   </si>
@@ -157,6 +157,21 @@
   </si>
   <si>
     <t>The term Ecology coined.</t>
+  </si>
+  <si>
+    <t>Austric people come to India.</t>
+  </si>
+  <si>
+    <t>Dravidians come to India.</t>
+  </si>
+  <si>
+    <t>Brahui (Dravidian) speakers come to India.</t>
+  </si>
+  <si>
+    <t>Start of the Middle Indo-Aryan, covering Prakrit, Pali, and Apabhramsha languages.</t>
+  </si>
+  <si>
+    <t>Oral legends and traditions of Munda and Tibeto-Burman languages recorded by Christian missionaries.</t>
   </si>
 </sst>
 </file>
@@ -474,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -851,6 +866,46 @@
         <v>43</v>
       </c>
     </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>-50000</v>
+      </c>
+      <c r="C42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>-30000</v>
+      </c>
+      <c r="C43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>-4000</v>
+      </c>
+      <c r="C44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>-500</v>
+      </c>
+      <c r="C45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>1800</v>
+      </c>
+      <c r="C46" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>